<commit_message>
including window wall ratios in all directions
This is also tackeld in issue #662 but i add it here so it is easy to
merge in the future
</commit_message>
<xml_diff>
--- a/cea/databases/archetypes/construction_properties_SIN.xlsx
+++ b/cea/databases/archetypes/construction_properties_SIN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\GitHub\CEAforArcGIS\cea\databases\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimeno\Documents\CEAforArcGIS\cea\databases\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="65">
   <si>
     <t>Code</t>
   </si>
@@ -50,9 +50,6 @@
     <t>type_ctrl</t>
   </si>
   <si>
-    <t>win_wall</t>
-  </si>
-  <si>
     <t>type_shade</t>
   </si>
   <si>
@@ -216,6 +213,18 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>wwr_north</t>
+  </si>
+  <si>
+    <t>wwr_south</t>
+  </si>
+  <si>
+    <t>wwr_east</t>
+  </si>
+  <si>
+    <t>wwr_west</t>
   </si>
 </sst>
 </file>
@@ -1099,79 +1108,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.59765625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.265625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="7.1328125" style="4" customWidth="1"/>
+    <col min="6" max="9" width="10.86328125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="11.73046875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.1328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="12.3984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" s="3">
         <v>0.25</v>
@@ -1179,38 +1197,47 @@
       <c r="F2" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="N2" s="11"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="11"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="3">
         <v>0.25</v>
@@ -1218,37 +1245,46 @@
       <c r="F3" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="3">
         <v>0.84</v>
@@ -1256,37 +1292,46 @@
       <c r="F4" s="3">
         <v>0.35</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="N4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="3">
         <v>0.84</v>
@@ -1294,37 +1339,46 @@
       <c r="F5" s="3">
         <v>0.35</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="3" t="s">
+      <c r="N5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="3">
         <v>0.84</v>
@@ -1332,37 +1386,46 @@
       <c r="F6" s="3">
         <v>0.35</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="N6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="3">
         <v>0.84</v>
@@ -1370,37 +1433,46 @@
       <c r="F7" s="3">
         <v>0</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="N7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="3">
         <v>0.84</v>
@@ -1408,37 +1480,46 @@
       <c r="F8" s="3">
         <v>0.35</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="N8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="3">
         <v>0.7</v>
@@ -1446,37 +1527,46 @@
       <c r="F9" s="3">
         <v>0.1</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I9" s="3" t="s">
+      <c r="N9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="3">
         <v>0.67</v>
@@ -1484,37 +1574,46 @@
       <c r="F10" s="3">
         <v>0.35</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" s="3">
         <v>0.84</v>
@@ -1522,37 +1621,46 @@
       <c r="F11" s="3">
         <v>0.35</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I11" s="3" t="s">
+      <c r="N11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="3">
         <v>0.67</v>
@@ -1560,75 +1668,93 @@
       <c r="F12" s="3">
         <v>0.35</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I12" s="3" t="s">
+      <c r="N12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K12" s="3" t="s">
+      <c r="M13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O13" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0.35</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I13" s="3" t="s">
+      <c r="C14" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
@@ -1636,37 +1762,46 @@
       <c r="F14" s="3">
         <v>0</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I14" s="3" t="s">
+      <c r="N14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="J14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="3">
         <v>0</v>
@@ -1674,37 +1809,46 @@
       <c r="F15" s="3">
         <v>0.5</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="N15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
@@ -1712,37 +1856,46 @@
       <c r="F16" s="3">
         <v>0</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J16" s="3" t="s">
+      <c r="N16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O16" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="3">
         <v>0.67</v>
@@ -1750,37 +1903,46 @@
       <c r="F17" s="3">
         <v>0.35</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J17" s="3" t="s">
+      <c r="N17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K17" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O17" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="3">
         <v>0.67</v>
@@ -1788,37 +1950,46 @@
       <c r="F18" s="3">
         <v>0.35</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J18" s="3" t="s">
+      <c r="N18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O18" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="3">
         <v>0.67</v>
@@ -1826,23 +1997,32 @@
       <c r="F19" s="3">
         <v>0.35</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J19" s="3" t="s">
+      <c r="N19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>51</v>
+      <c r="O19" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1862,31 +2042,31 @@
       <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="13" customWidth="1"/>
+    <col min="1" max="1" width="12.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="12.73046875" style="13" customWidth="1"/>
     <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="6" width="9.1328125" style="4"/>
+    <col min="7" max="7" width="9.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.265625" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -1901,532 +2081,532 @@
         <v>5</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="C17" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="G17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="G18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="C19" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="G19" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1048576" spans="8:8" x14ac:dyDescent="0.45">
       <c r="H1048576" s="3"/>
     </row>
   </sheetData>
@@ -2443,40 +2623,40 @@
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.3984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.86328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.86328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.73046875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="8">
         <v>24</v>
@@ -2494,9 +2674,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="8">
         <v>24</v>
@@ -2514,9 +2694,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="8">
         <v>24</v>
@@ -2534,9 +2714,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="8">
         <v>24</v>
@@ -2554,9 +2734,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="8">
         <v>24</v>
@@ -2574,9 +2754,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="8">
         <v>24</v>
@@ -2594,9 +2774,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="8">
         <v>24</v>
@@ -2615,9 +2795,9 @@
         <v>25.15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="8">
         <v>24</v>
@@ -2635,9 +2815,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="8">
         <v>24</v>
@@ -2655,9 +2835,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="8">
         <v>24</v>
@@ -2675,9 +2855,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="8">
         <v>24</v>
@@ -2695,9 +2875,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="8">
         <v>50</v>
@@ -2715,9 +2895,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="8">
         <v>24</v>
@@ -2735,29 +2915,29 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="8">
+        <v>50</v>
+      </c>
+      <c r="C15" s="5">
+        <v>10</v>
+      </c>
+      <c r="D15" s="5">
+        <v>50</v>
+      </c>
+      <c r="E15" s="5">
+        <v>10</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" s="8">
-        <v>50</v>
-      </c>
-      <c r="C15" s="5">
-        <v>10</v>
-      </c>
-      <c r="D15" s="5">
-        <v>50</v>
-      </c>
-      <c r="E15" s="5">
-        <v>10</v>
-      </c>
-      <c r="F15" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="B16" s="8">
         <v>-5</v>
@@ -2775,9 +2955,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="8">
         <v>24</v>
@@ -2796,9 +2976,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="8">
         <v>24</v>
@@ -2816,9 +2996,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="8">
         <v>24</v>
@@ -2850,55 +3030,55 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="15.3984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.3984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1328125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="G1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="I1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2" s="6" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="B2" s="8">
         <v>70</v>
@@ -2928,9 +3108,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="5">
         <v>70</v>
@@ -2960,9 +3140,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="8">
         <v>70</v>
@@ -2992,9 +3172,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="8">
         <v>70</v>
@@ -3024,9 +3204,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="8">
         <v>70</v>
@@ -3056,9 +3236,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="8">
         <v>70</v>
@@ -3088,9 +3268,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="8">
         <v>73</v>
@@ -3120,9 +3300,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="8">
         <v>90</v>
@@ -3152,9 +3332,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="8">
         <v>70</v>
@@ -3184,9 +3364,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="8">
         <v>70</v>
@@ -3216,9 +3396,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="8">
         <v>110</v>
@@ -3248,9 +3428,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="8">
         <v>70</v>
@@ -3280,9 +3460,9 @@
         <v>360</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="8">
         <v>0</v>
@@ -3312,9 +3492,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="8">
         <v>0</v>
@@ -3344,9 +3524,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="8">
         <v>0</v>
@@ -3376,9 +3556,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="8">
         <f>B11</f>
@@ -3411,9 +3591,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="8">
         <v>70</v>
@@ -3443,9 +3623,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="8">
         <v>70</v>
@@ -3475,7 +3655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="G22" s="12"/>
     </row>
   </sheetData>

</xml_diff>